<commit_message>
chongryang 2020 - deleted 7 10
</commit_message>
<xml_diff>
--- a/data/han/총량/가평천3_2020.xlsx
+++ b/data/han/총량/가평천3_2020.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\사업관련\환경AI\모듈작업\water-quality\data\han\총량\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="132">
   <si>
     <t>dt</t>
   </si>
@@ -408,102 +415,38 @@
   </si>
   <si>
     <t>20200708</t>
-  </si>
-  <si>
-    <t>2020-07-15 12:00</t>
-  </si>
-  <si>
-    <t>20200715</t>
-  </si>
-  <si>
-    <t>2020-07-20 12:00</t>
-  </si>
-  <si>
-    <t>20200722</t>
-  </si>
-  <si>
-    <t>2020-07-25 12:00</t>
-  </si>
-  <si>
-    <t>20200729</t>
-  </si>
-  <si>
-    <t>2020-08-06 12:00</t>
-  </si>
-  <si>
-    <t>20200803</t>
-  </si>
-  <si>
-    <t>2020-08-12 12:00</t>
-  </si>
-  <si>
-    <t>20200810</t>
-  </si>
-  <si>
-    <t>2020-08-18 12:00</t>
-  </si>
-  <si>
-    <t>20200820</t>
-  </si>
-  <si>
-    <t>2020-08-24 12:00</t>
-  </si>
-  <si>
-    <t>20200826</t>
-  </si>
-  <si>
-    <t>2020-09-05 12:00</t>
-  </si>
-  <si>
-    <t>20200902</t>
-  </si>
-  <si>
-    <t>2020-09-10 12:00</t>
-  </si>
-  <si>
-    <t>20200909</t>
-  </si>
-  <si>
-    <t>2020-09-15 12:00</t>
-  </si>
-  <si>
-    <t>20200917</t>
-  </si>
-  <si>
-    <t>2020-09-20 12:00</t>
-  </si>
-  <si>
-    <t>20200923</t>
-  </si>
-  <si>
-    <t>2020-09-25 12:00</t>
-  </si>
-  <si>
-    <t>20200928</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="0.00000"/>
+    <numFmt numFmtId="178" formatCode="0.000"/>
+    <numFmt numFmtId="179" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -521,7 +464,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -529,17 +478,25 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -548,10 +505,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -797,83 +754,84 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:BJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD40"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.43" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.86" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.57" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.71" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.75" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.75" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.75" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.43" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.75" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.43" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.71" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.75" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.75" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.71" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.71" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.71" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.75" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.71" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.14" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.29" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.29" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.57" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.29" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.29" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.29" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.57" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="10" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.14" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.29" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.71" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.43" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.43" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.43" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.71" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.43" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.86" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14.29" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="16" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="16" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="13" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="16" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="13" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14.29" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.71" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.86" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1019,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1138,7 +1096,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1218,19 +1176,19 @@
         <v>1.855</v>
       </c>
       <c r="AD3" s="5">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="AE3" s="5">
-        <v>7.7999999999999998</v>
+        <v>7.8</v>
       </c>
       <c r="AF3">
         <v>15</v>
       </c>
       <c r="AG3" s="5">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="AH3" s="5">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="AI3" s="5">
         <v>1.2</v>
@@ -1245,28 +1203,28 @@
         <v>2.4550000000000001</v>
       </c>
       <c r="AM3" s="5">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="AN3" s="4">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AO3" s="4">
-        <v>0.0060000000000000001</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AP3" s="4">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AQ3" s="4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AR3" s="5">
-        <v>6.9000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="AS3" s="5">
-        <v>0.69999999999999996</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -1343,7 +1301,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -1420,7 +1378,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -1497,7 +1455,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1574,7 +1532,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -1654,7 +1612,7 @@
         <v>0.88900000000000001</v>
       </c>
       <c r="AD8" s="5">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="AE8" s="5">
         <v>8.1999999999999993</v>
@@ -1663,13 +1621,13 @@
         <v>13.6</v>
       </c>
       <c r="AG8" s="5">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="AH8" s="5">
         <v>1.8</v>
       </c>
       <c r="AI8" s="5">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="AJ8">
         <v>95</v>
@@ -1684,25 +1642,25 @@
         <v>1.976</v>
       </c>
       <c r="AN8" s="4">
-        <v>0.0089999999999999993</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AO8" s="4">
-        <v>0.0040000000000000001</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AP8" s="4">
-        <v>0.0030000000000000001</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AQ8" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AR8" s="5">
         <v>1.1000000000000001</v>
       </c>
       <c r="AS8" s="5">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -1779,7 +1737,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -1862,13 +1820,13 @@
         <v>7.5</v>
       </c>
       <c r="AE10" s="5">
-        <v>8.0999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="AF10">
         <v>13</v>
       </c>
       <c r="AG10" s="5">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="AH10" s="5">
         <v>1.8</v>
@@ -1889,22 +1847,22 @@
         <v>1.74</v>
       </c>
       <c r="AN10" s="4">
-        <v>0.0080000000000000002</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AO10" s="4">
-        <v>0.0070000000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AP10" s="4">
-        <v>0.0040000000000000001</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AQ10" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AS10" s="5">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -1990,7 +1948,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="AF11" s="5">
-        <v>12.300000000000001</v>
+        <v>12.3</v>
       </c>
       <c r="AG11" s="5">
         <v>0.5</v>
@@ -2014,25 +1972,25 @@
         <v>1.629</v>
       </c>
       <c r="AN11" s="4">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AO11" s="4">
-        <v>0.0080000000000000002</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AP11" s="4">
-        <v>0.0060000000000000001</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AQ11">
         <v>0</v>
       </c>
       <c r="AR11" s="5">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="AS11" s="5">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -2112,7 +2070,7 @@
         <v>1.022</v>
       </c>
       <c r="AD12" s="5">
-        <v>7.7999999999999998</v>
+        <v>7.8</v>
       </c>
       <c r="AE12" s="5">
         <v>8.1999999999999993</v>
@@ -2121,13 +2079,13 @@
         <v>12.5</v>
       </c>
       <c r="AG12" s="5">
-        <v>0.59999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="AH12" s="5">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="AI12" s="5">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="AJ12">
         <v>76</v>
@@ -2136,28 +2094,28 @@
         <v>1.8819999999999999</v>
       </c>
       <c r="AL12" s="6">
-        <v>1.8700000000000001</v>
+        <v>1.87</v>
       </c>
       <c r="AM12" s="6">
         <v>1.73</v>
       </c>
       <c r="AN12" s="4">
-        <v>0.017000000000000001</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AO12" s="4">
-        <v>0.0060000000000000001</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AP12" s="4">
-        <v>0.0030000000000000001</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AQ12" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AS12" s="5">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -2249,10 +2207,10 @@
         <v>1</v>
       </c>
       <c r="AH13" s="5">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="AI13" s="5">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="AJ13">
         <v>77</v>
@@ -2267,22 +2225,22 @@
         <v>1.542</v>
       </c>
       <c r="AN13" s="4">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AO13" s="4">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AP13" s="4">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AQ13" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AS13">
         <v>1</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -2362,22 +2320,22 @@
         <v>1.0189999999999999</v>
       </c>
       <c r="AD14" s="5">
-        <v>14.699999999999999</v>
+        <v>14.7</v>
       </c>
       <c r="AE14" s="5">
-        <v>8.0999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="AF14" s="5">
         <v>10.5</v>
       </c>
       <c r="AG14" s="5">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="AH14" s="5">
         <v>2.2000000000000002</v>
       </c>
       <c r="AI14" s="5">
-        <v>4.2999999999999998</v>
+        <v>4.3</v>
       </c>
       <c r="AJ14">
         <v>78</v>
@@ -2392,22 +2350,22 @@
         <v>1.6180000000000001</v>
       </c>
       <c r="AN14" s="4">
-        <v>0.028000000000000001</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="AO14" s="4">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="AP14" s="4">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AQ14" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AS14">
         <v>1</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -2496,13 +2454,13 @@
         <v>10.5</v>
       </c>
       <c r="AG15" s="5">
-        <v>0.69999999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="AH15" s="5">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="AI15" s="5">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="AJ15">
         <v>86</v>
@@ -2517,22 +2475,22 @@
         <v>1.645</v>
       </c>
       <c r="AN15" s="4">
-        <v>0.033000000000000002</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="AO15" s="4">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AP15" s="4">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AQ15" s="4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AS15">
         <v>1</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -2615,7 +2573,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="AE16" s="5">
-        <v>8.5999999999999996</v>
+        <v>8.6</v>
       </c>
       <c r="AF16" s="5">
         <v>11.5</v>
@@ -2624,10 +2582,10 @@
         <v>1</v>
       </c>
       <c r="AH16" s="5">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="AI16" s="5">
-        <v>3.7000000000000002</v>
+        <v>3.7</v>
       </c>
       <c r="AJ16">
         <v>97</v>
@@ -2642,25 +2600,25 @@
         <v>1.6859999999999999</v>
       </c>
       <c r="AN16" s="4">
-        <v>0.035999999999999997</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="AO16" s="4">
-        <v>0.014999999999999999</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AP16" s="4">
-        <v>0.0060000000000000001</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AQ16" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AR16" s="5">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="AS16" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -2740,22 +2698,22 @@
         <v>1.161</v>
       </c>
       <c r="AD17" s="5">
-        <v>12.699999999999999</v>
+        <v>12.7</v>
       </c>
       <c r="AE17" s="5">
-        <v>8.4000000000000004</v>
+        <v>8.4</v>
       </c>
       <c r="AF17" s="5">
         <v>11.4</v>
       </c>
       <c r="AG17" s="5">
-        <v>0.69999999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="AH17" s="5">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="AI17" s="5">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="AJ17">
         <v>88</v>
@@ -2773,19 +2731,19 @@
         <v>0.02</v>
       </c>
       <c r="AO17" s="4">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AP17" s="4">
-        <v>0.0060000000000000001</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AQ17" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AS17">
         <v>1</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -2865,7 +2823,7 @@
         <v>0.47899999999999998</v>
       </c>
       <c r="AD18" s="5">
-        <v>18.300000000000001</v>
+        <v>18.3</v>
       </c>
       <c r="AE18" s="5">
         <v>8.8000000000000007</v>
@@ -2877,10 +2835,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AH18" s="5">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="AI18" s="5">
-        <v>3.7000000000000002</v>
+        <v>3.7</v>
       </c>
       <c r="AJ18">
         <v>94</v>
@@ -2895,22 +2853,22 @@
         <v>1.5640000000000001</v>
       </c>
       <c r="AN18" s="4">
-        <v>0.025999999999999999</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="AO18" s="4">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AP18" s="4">
-        <v>0.0080000000000000002</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AQ18" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AS18" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -2990,19 +2948,19 @@
         <v>0.219</v>
       </c>
       <c r="AD19" s="5">
-        <v>23.100000000000001</v>
+        <v>23.1</v>
       </c>
       <c r="AE19" s="5">
-        <v>9.0999999999999996</v>
+        <v>9.1</v>
       </c>
       <c r="AF19" s="5">
-        <v>11.699999999999999</v>
+        <v>11.7</v>
       </c>
       <c r="AG19" s="5">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="AH19" s="5">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="AI19" s="5">
         <v>8.1999999999999993</v>
@@ -3014,28 +2972,28 @@
         <v>1.768</v>
       </c>
       <c r="AL19" s="6">
-        <v>1.6699999999999999</v>
+        <v>1.67</v>
       </c>
       <c r="AM19" s="4">
         <v>1.4570000000000001</v>
       </c>
       <c r="AN19" s="4">
-        <v>0.045999999999999999</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="AO19" s="4">
-        <v>0.035999999999999997</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="AP19" s="6">
         <v>0.01</v>
       </c>
       <c r="AQ19" s="4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AS19" s="5">
         <v>1.7</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>114</v>
       </c>
@@ -3124,13 +3082,13 @@
         <v>12</v>
       </c>
       <c r="AG20" s="5">
-        <v>0.69999999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="AH20" s="5">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="AI20" s="5">
-        <v>15.300000000000001</v>
+        <v>15.3</v>
       </c>
       <c r="AJ20">
         <v>74</v>
@@ -3145,16 +3103,16 @@
         <v>1.742</v>
       </c>
       <c r="AN20" s="4">
-        <v>0.017000000000000001</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AO20" s="4">
-        <v>0.024</v>
+        <v>2.4E-2</v>
       </c>
       <c r="AP20" s="4">
-        <v>0.0089999999999999993</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AQ20" s="4">
-        <v>0.0030000000000000001</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AR20" s="5">
         <v>1.5</v>
@@ -3163,7 +3121,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -3249,16 +3207,16 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="AF21" s="5">
-        <v>11.300000000000001</v>
+        <v>11.3</v>
       </c>
       <c r="AG21" s="5">
         <v>0.5</v>
       </c>
       <c r="AH21" s="5">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="AI21" s="5">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="AJ21">
         <v>59</v>
@@ -3273,22 +3231,22 @@
         <v>2.0529999999999999</v>
       </c>
       <c r="AN21" s="4">
-        <v>0.010999999999999999</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="AO21" s="4">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="AP21" s="4">
-        <v>0.0070000000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AQ21" s="4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AS21" s="5">
         <v>1.2</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>118</v>
       </c>
@@ -3365,22 +3323,22 @@
         <v>119</v>
       </c>
       <c r="AC22" s="6">
-        <v>7.7400000000000002</v>
+        <v>7.74</v>
       </c>
       <c r="AD22" s="5">
-        <v>20.199999999999999</v>
+        <v>20.2</v>
       </c>
       <c r="AE22">
         <v>8</v>
       </c>
       <c r="AF22" s="5">
-        <v>9.9000000000000004</v>
+        <v>9.9</v>
       </c>
       <c r="AG22" s="5">
-        <v>0.59999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="AH22" s="5">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="AI22" s="5">
         <v>2.2000000000000002</v>
@@ -3398,22 +3356,22 @@
         <v>1.5920000000000001</v>
       </c>
       <c r="AN22" s="4">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="AO22" s="4">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="AP22" s="4">
-        <v>0.0080000000000000002</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AQ22" s="4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AS22">
         <v>1</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -3493,7 +3451,7 @@
         <v>2.8780000000000001</v>
       </c>
       <c r="AD23" s="5">
-        <v>24.199999999999999</v>
+        <v>24.2</v>
       </c>
       <c r="AE23" s="5">
         <v>8.1999999999999993</v>
@@ -3502,7 +3460,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="AG23" s="5">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="AH23" s="5">
         <v>2.5</v>
@@ -3523,22 +3481,22 @@
         <v>1.5289999999999999</v>
       </c>
       <c r="AN23" s="4">
-        <v>0.037999999999999999</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="AO23" s="4">
-        <v>0.017000000000000001</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AP23" s="6">
         <v>0.01</v>
       </c>
       <c r="AQ23" s="4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AS23" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>122</v>
       </c>
@@ -3618,22 +3576,22 @@
         <v>1.3089999999999999</v>
       </c>
       <c r="AD24" s="5">
-        <v>28.899999999999999</v>
+        <v>28.9</v>
       </c>
       <c r="AE24" s="5">
-        <v>8.4000000000000004</v>
+        <v>8.4</v>
       </c>
       <c r="AF24">
         <v>9</v>
       </c>
       <c r="AG24" s="5">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="AH24" s="5">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="AI24" s="5">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="AJ24">
         <v>118</v>
@@ -3648,25 +3606,25 @@
         <v>1.3660000000000001</v>
       </c>
       <c r="AN24" s="4">
-        <v>0.021999999999999999</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="AO24" s="4">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AP24" s="4">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AQ24" s="4">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AR24" s="5">
-        <v>5.9000000000000004</v>
+        <v>5.9</v>
       </c>
       <c r="AS24" s="5">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -3758,7 +3716,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AH25" s="5">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="AI25" s="5">
         <v>3.5</v>
@@ -3776,22 +3734,22 @@
         <v>1.1579999999999999</v>
       </c>
       <c r="AN25" s="4">
-        <v>0.021999999999999999</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="AO25" s="4">
-        <v>0.025000000000000001</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AP25" s="4">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AQ25" s="4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AS25" s="5">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>126</v>
       </c>
@@ -3871,22 +3829,22 @@
         <v>1.3140000000000001</v>
       </c>
       <c r="AD26" s="5">
-        <v>23.199999999999999</v>
+        <v>23.2</v>
       </c>
       <c r="AE26" s="5">
-        <v>7.9000000000000004</v>
+        <v>7.9</v>
       </c>
       <c r="AF26" s="5">
-        <v>8.4000000000000004</v>
+        <v>8.4</v>
       </c>
       <c r="AG26">
         <v>1</v>
       </c>
       <c r="AH26" s="5">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="AI26" s="5">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
       <c r="AJ26">
         <v>141</v>
@@ -3901,22 +3859,22 @@
         <v>1.052</v>
       </c>
       <c r="AN26" s="4">
-        <v>0.029000000000000001</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="AO26" s="4">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AP26" s="4">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="AQ26" s="4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AS26" s="5">
         <v>1.7</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -3996,7 +3954,7 @@
         <v>5.3449999999999998</v>
       </c>
       <c r="AD27" s="5">
-        <v>24.800000000000001</v>
+        <v>24.8</v>
       </c>
       <c r="AE27">
         <v>8</v>
@@ -4005,13 +3963,13 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="AG27" s="5">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="AH27" s="5">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AI27" s="5">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="AJ27">
         <v>89</v>
@@ -4026,22 +3984,22 @@
         <v>1.1639999999999999</v>
       </c>
       <c r="AN27" s="4">
-        <v>0.0089999999999999993</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AO27" s="4">
-        <v>0.017000000000000001</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AP27" s="6">
         <v>0.01</v>
       </c>
       <c r="AQ27" s="4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AS27" s="5">
         <v>1.7</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -4121,22 +4079,22 @@
         <v>1.5289999999999999</v>
       </c>
       <c r="AD28" s="5">
-        <v>28.300000000000001</v>
+        <v>28.3</v>
       </c>
       <c r="AE28" s="5">
         <v>8.3000000000000007</v>
       </c>
       <c r="AF28" s="5">
-        <v>9.0999999999999996</v>
+        <v>9.1</v>
       </c>
       <c r="AG28" s="5">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="AH28">
         <v>3</v>
       </c>
       <c r="AI28" s="5">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="AJ28">
         <v>119</v>
@@ -4151,1387 +4109,23 @@
         <v>1.02</v>
       </c>
       <c r="AN28" s="4">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="AO28" s="4">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="AP28" s="4">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AQ28" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AS28" s="5">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F29" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G29" t="s">
-        <v>66</v>
-      </c>
-      <c r="H29" t="s">
-        <v>67</v>
-      </c>
-      <c r="L29" t="s">
-        <v>66</v>
-      </c>
-      <c r="M29" t="s">
-        <v>67</v>
-      </c>
-      <c r="N29" t="s">
-        <v>68</v>
-      </c>
-      <c r="O29" t="s">
-        <v>69</v>
-      </c>
-      <c r="P29" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>71</v>
-      </c>
-      <c r="R29" t="s">
-        <v>72</v>
-      </c>
-      <c r="S29" t="s">
-        <v>73</v>
-      </c>
-      <c r="T29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U29" t="s">
-        <v>74</v>
-      </c>
-      <c r="V29" t="s">
-        <v>68</v>
-      </c>
-      <c r="W29" t="s">
-        <v>69</v>
-      </c>
-      <c r="X29" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC29" s="4">
-        <v>7.9960000000000004</v>
-      </c>
-      <c r="AD29" s="5">
-        <v>22.100000000000001</v>
-      </c>
-      <c r="AE29" s="5">
-        <v>7.9000000000000004</v>
-      </c>
-      <c r="AF29" s="5">
-        <v>9.5999999999999996</v>
-      </c>
-      <c r="AG29" s="5">
-        <v>0.69999999999999996</v>
-      </c>
-      <c r="AH29" s="5">
-        <v>3.1000000000000001</v>
-      </c>
-      <c r="AI29" s="5">
-        <v>2.1000000000000001</v>
-      </c>
-      <c r="AJ29">
-        <v>86</v>
-      </c>
-      <c r="AK29" s="4">
-        <v>1.415</v>
-      </c>
-      <c r="AL29" s="5">
-        <v>1.3999999999999999</v>
-      </c>
-      <c r="AM29" s="4">
-        <v>1.331</v>
-      </c>
-      <c r="AN29" s="4">
-        <v>0.0080000000000000002</v>
-      </c>
-      <c r="AO29" s="4">
-        <v>0.016</v>
-      </c>
-      <c r="AP29" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="AQ29" s="4">
-        <v>0.0040000000000000001</v>
-      </c>
-      <c r="AR29" s="5">
-        <v>1.3999999999999999</v>
-      </c>
-      <c r="AS29" s="5">
-        <v>1.3999999999999999</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F30" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G30" t="s">
-        <v>66</v>
-      </c>
-      <c r="H30" t="s">
-        <v>67</v>
-      </c>
-      <c r="L30" t="s">
-        <v>66</v>
-      </c>
-      <c r="M30" t="s">
-        <v>67</v>
-      </c>
-      <c r="N30" t="s">
-        <v>68</v>
-      </c>
-      <c r="O30" t="s">
-        <v>69</v>
-      </c>
-      <c r="P30" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>71</v>
-      </c>
-      <c r="R30" t="s">
-        <v>72</v>
-      </c>
-      <c r="S30" t="s">
-        <v>73</v>
-      </c>
-      <c r="T30" t="s">
-        <v>74</v>
-      </c>
-      <c r="U30" t="s">
-        <v>74</v>
-      </c>
-      <c r="V30" t="s">
-        <v>68</v>
-      </c>
-      <c r="W30" t="s">
-        <v>69</v>
-      </c>
-      <c r="X30" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>135</v>
-      </c>
-      <c r="AC30" s="4">
-        <v>6.9669999999999996</v>
-      </c>
-      <c r="AD30" s="5">
-        <v>23.300000000000001</v>
-      </c>
-      <c r="AE30" s="5">
-        <v>7.7999999999999998</v>
-      </c>
-      <c r="AF30" s="5">
-        <v>9.4000000000000004</v>
-      </c>
-      <c r="AG30" s="5">
-        <v>0.59999999999999998</v>
-      </c>
-      <c r="AH30" s="5">
-        <v>3.1000000000000001</v>
-      </c>
-      <c r="AI30" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="AJ30">
-        <v>82</v>
-      </c>
-      <c r="AK30" s="4">
-        <v>1.341</v>
-      </c>
-      <c r="AL30" s="4">
-        <v>1.319</v>
-      </c>
-      <c r="AM30" s="4">
-        <v>1.226</v>
-      </c>
-      <c r="AN30" s="4">
-        <v>0.012</v>
-      </c>
-      <c r="AO30" s="4">
-        <v>0.012</v>
-      </c>
-      <c r="AP30" s="4">
-        <v>0.0060000000000000001</v>
-      </c>
-      <c r="AQ30" s="4">
-        <v>0.0050000000000000001</v>
-      </c>
-      <c r="AS30" s="5">
-        <v>1.6000000000000001</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>136</v>
-      </c>
-      <c r="B31" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F31" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G31" t="s">
-        <v>66</v>
-      </c>
-      <c r="H31" t="s">
-        <v>67</v>
-      </c>
-      <c r="L31" t="s">
-        <v>66</v>
-      </c>
-      <c r="M31" t="s">
-        <v>67</v>
-      </c>
-      <c r="N31" t="s">
-        <v>68</v>
-      </c>
-      <c r="O31" t="s">
-        <v>69</v>
-      </c>
-      <c r="P31" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>71</v>
-      </c>
-      <c r="R31" t="s">
-        <v>72</v>
-      </c>
-      <c r="S31" t="s">
-        <v>73</v>
-      </c>
-      <c r="T31" t="s">
-        <v>74</v>
-      </c>
-      <c r="U31" t="s">
-        <v>74</v>
-      </c>
-      <c r="V31" t="s">
-        <v>68</v>
-      </c>
-      <c r="W31" t="s">
-        <v>69</v>
-      </c>
-      <c r="X31" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>137</v>
-      </c>
-      <c r="AC31" s="4">
-        <v>18.161000000000001</v>
-      </c>
-      <c r="AD31" s="5">
-        <v>20.300000000000001</v>
-      </c>
-      <c r="AE31" s="5">
-        <v>7.9000000000000004</v>
-      </c>
-      <c r="AF31" s="5">
-        <v>10.6</v>
-      </c>
-      <c r="AG31" s="5">
-        <v>0.40000000000000002</v>
-      </c>
-      <c r="AH31">
-        <v>3</v>
-      </c>
-      <c r="AI31" s="5">
-        <v>3.5</v>
-      </c>
-      <c r="AJ31">
-        <v>86</v>
-      </c>
-      <c r="AK31" s="4">
-        <v>1.948</v>
-      </c>
-      <c r="AL31" s="6">
-        <v>1.9199999999999999</v>
-      </c>
-      <c r="AM31" s="4">
-        <v>1.792</v>
-      </c>
-      <c r="AN31" s="4">
-        <v>0.019</v>
-      </c>
-      <c r="AO31" s="4">
-        <v>0.027</v>
-      </c>
-      <c r="AP31" s="4">
-        <v>0.017999999999999999</v>
-      </c>
-      <c r="AQ31" s="4">
-        <v>0.010999999999999999</v>
-      </c>
-      <c r="AS31" s="5">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>138</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F32" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G32" t="s">
-        <v>66</v>
-      </c>
-      <c r="H32" t="s">
-        <v>67</v>
-      </c>
-      <c r="L32" t="s">
-        <v>66</v>
-      </c>
-      <c r="M32" t="s">
-        <v>67</v>
-      </c>
-      <c r="N32" t="s">
-        <v>68</v>
-      </c>
-      <c r="O32" t="s">
-        <v>69</v>
-      </c>
-      <c r="P32" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>71</v>
-      </c>
-      <c r="R32" t="s">
-        <v>72</v>
-      </c>
-      <c r="S32" t="s">
-        <v>73</v>
-      </c>
-      <c r="T32" t="s">
-        <v>74</v>
-      </c>
-      <c r="U32" t="s">
-        <v>74</v>
-      </c>
-      <c r="V32" t="s">
-        <v>68</v>
-      </c>
-      <c r="W32" t="s">
-        <v>69</v>
-      </c>
-      <c r="X32" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>140</v>
-      </c>
-      <c r="B33" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F33" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G33" t="s">
-        <v>66</v>
-      </c>
-      <c r="H33" t="s">
-        <v>67</v>
-      </c>
-      <c r="L33" t="s">
-        <v>66</v>
-      </c>
-      <c r="M33" t="s">
-        <v>67</v>
-      </c>
-      <c r="N33" t="s">
-        <v>68</v>
-      </c>
-      <c r="O33" t="s">
-        <v>69</v>
-      </c>
-      <c r="P33" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>71</v>
-      </c>
-      <c r="R33" t="s">
-        <v>72</v>
-      </c>
-      <c r="S33" t="s">
-        <v>73</v>
-      </c>
-      <c r="T33" t="s">
-        <v>74</v>
-      </c>
-      <c r="U33" t="s">
-        <v>74</v>
-      </c>
-      <c r="V33" t="s">
-        <v>68</v>
-      </c>
-      <c r="W33" t="s">
-        <v>69</v>
-      </c>
-      <c r="X33" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>142</v>
-      </c>
-      <c r="B34" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F34" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H34" t="s">
-        <v>67</v>
-      </c>
-      <c r="L34" t="s">
-        <v>66</v>
-      </c>
-      <c r="M34" t="s">
-        <v>67</v>
-      </c>
-      <c r="N34" t="s">
-        <v>68</v>
-      </c>
-      <c r="O34" t="s">
-        <v>69</v>
-      </c>
-      <c r="P34" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>71</v>
-      </c>
-      <c r="R34" t="s">
-        <v>72</v>
-      </c>
-      <c r="S34" t="s">
-        <v>73</v>
-      </c>
-      <c r="T34" t="s">
-        <v>74</v>
-      </c>
-      <c r="U34" t="s">
-        <v>74</v>
-      </c>
-      <c r="V34" t="s">
-        <v>68</v>
-      </c>
-      <c r="W34" t="s">
-        <v>69</v>
-      </c>
-      <c r="X34" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>143</v>
-      </c>
-      <c r="AC34" s="4">
-        <v>8.8119999999999994</v>
-      </c>
-      <c r="AD34" s="5">
-        <v>20.5</v>
-      </c>
-      <c r="AE34" s="5">
-        <v>7.5999999999999996</v>
-      </c>
-      <c r="AF34" s="5">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="AG34" s="5">
-        <v>0.69999999999999996</v>
-      </c>
-      <c r="AH34" s="5">
-        <v>3.1000000000000001</v>
-      </c>
-      <c r="AI34" s="5">
-        <v>0.80000000000000004</v>
-      </c>
-      <c r="AJ34">
-        <v>83</v>
-      </c>
-      <c r="AK34" s="4">
-        <v>1.798</v>
-      </c>
-      <c r="AL34" s="4">
-        <v>1.7829999999999999</v>
-      </c>
-      <c r="AM34" s="4">
-        <v>1.6439999999999999</v>
-      </c>
-      <c r="AN34" s="4">
-        <v>0.0089999999999999993</v>
-      </c>
-      <c r="AO34" s="4">
-        <v>0.012999999999999999</v>
-      </c>
-      <c r="AP34" s="4">
-        <v>0.0089999999999999993</v>
-      </c>
-      <c r="AQ34" s="4">
-        <v>0.002</v>
-      </c>
-      <c r="AR34" s="5">
-        <v>1.6000000000000001</v>
-      </c>
-      <c r="AS34" s="5">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>144</v>
-      </c>
-      <c r="B35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F35" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G35" t="s">
-        <v>66</v>
-      </c>
-      <c r="H35" t="s">
-        <v>67</v>
-      </c>
-      <c r="L35" t="s">
-        <v>66</v>
-      </c>
-      <c r="M35" t="s">
-        <v>67</v>
-      </c>
-      <c r="N35" t="s">
-        <v>68</v>
-      </c>
-      <c r="O35" t="s">
-        <v>69</v>
-      </c>
-      <c r="P35" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>71</v>
-      </c>
-      <c r="R35" t="s">
-        <v>72</v>
-      </c>
-      <c r="S35" t="s">
-        <v>73</v>
-      </c>
-      <c r="T35" t="s">
-        <v>74</v>
-      </c>
-      <c r="U35" t="s">
-        <v>74</v>
-      </c>
-      <c r="V35" t="s">
-        <v>68</v>
-      </c>
-      <c r="W35" t="s">
-        <v>69</v>
-      </c>
-      <c r="X35" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z35" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC35" s="4">
-        <v>6.0510000000000002</v>
-      </c>
-      <c r="AD35" s="5">
-        <v>28.5</v>
-      </c>
-      <c r="AE35">
-        <v>8</v>
-      </c>
-      <c r="AF35" s="5">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="AG35" s="5">
-        <v>0.59999999999999998</v>
-      </c>
-      <c r="AH35" s="5">
-        <v>2.7000000000000002</v>
-      </c>
-      <c r="AI35" s="5">
-        <v>0.59999999999999998</v>
-      </c>
-      <c r="AJ35">
-        <v>97</v>
-      </c>
-      <c r="AK35" s="4">
-        <v>1.5840000000000001</v>
-      </c>
-      <c r="AL35" s="4">
-        <v>1.5720000000000001</v>
-      </c>
-      <c r="AM35" s="4">
-        <v>1.415</v>
-      </c>
-      <c r="AN35" s="4">
-        <v>0.024</v>
-      </c>
-      <c r="AO35" s="4">
-        <v>0.014</v>
-      </c>
-      <c r="AP35" s="4">
-        <v>0.0070000000000000001</v>
-      </c>
-      <c r="AQ35" s="4">
-        <v>0.002</v>
-      </c>
-      <c r="AS35" s="5">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>146</v>
-      </c>
-      <c r="B36" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F36" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G36" t="s">
-        <v>66</v>
-      </c>
-      <c r="H36" t="s">
-        <v>67</v>
-      </c>
-      <c r="L36" t="s">
-        <v>66</v>
-      </c>
-      <c r="M36" t="s">
-        <v>67</v>
-      </c>
-      <c r="N36" t="s">
-        <v>68</v>
-      </c>
-      <c r="O36" t="s">
-        <v>69</v>
-      </c>
-      <c r="P36" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>71</v>
-      </c>
-      <c r="R36" t="s">
-        <v>72</v>
-      </c>
-      <c r="S36" t="s">
-        <v>73</v>
-      </c>
-      <c r="T36" t="s">
-        <v>74</v>
-      </c>
-      <c r="U36" t="s">
-        <v>74</v>
-      </c>
-      <c r="V36" t="s">
-        <v>68</v>
-      </c>
-      <c r="W36" t="s">
-        <v>69</v>
-      </c>
-      <c r="X36" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z36" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC36" s="4">
-        <v>14.178000000000001</v>
-      </c>
-      <c r="AD36" s="5">
-        <v>23.199999999999999</v>
-      </c>
-      <c r="AE36" s="5">
-        <v>7.7000000000000002</v>
-      </c>
-      <c r="AF36" s="5">
-        <v>9.4000000000000004</v>
-      </c>
-      <c r="AG36" s="5">
-        <v>0.80000000000000004</v>
-      </c>
-      <c r="AH36" s="5">
-        <v>2.7000000000000002</v>
-      </c>
-      <c r="AI36" s="5">
-        <v>1.6000000000000001</v>
-      </c>
-      <c r="AJ36">
-        <v>78</v>
-      </c>
-      <c r="AK36" s="4">
-        <v>1.4359999999999999</v>
-      </c>
-      <c r="AL36" s="4">
-        <v>1.3959999999999999</v>
-      </c>
-      <c r="AM36" s="4">
-        <v>1.363</v>
-      </c>
-      <c r="AN36" s="4">
-        <v>0.023</v>
-      </c>
-      <c r="AO36" s="4">
-        <v>0.014999999999999999</v>
-      </c>
-      <c r="AP36" s="4">
-        <v>0.0070000000000000001</v>
-      </c>
-      <c r="AQ36" s="4">
-        <v>0.002</v>
-      </c>
-      <c r="AS36" s="5">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>148</v>
-      </c>
-      <c r="B37" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F37" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L37" t="s">
-        <v>66</v>
-      </c>
-      <c r="M37" t="s">
-        <v>67</v>
-      </c>
-      <c r="N37" t="s">
-        <v>68</v>
-      </c>
-      <c r="O37" t="s">
-        <v>69</v>
-      </c>
-      <c r="P37" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>71</v>
-      </c>
-      <c r="R37" t="s">
-        <v>72</v>
-      </c>
-      <c r="S37" t="s">
-        <v>73</v>
-      </c>
-      <c r="T37" t="s">
-        <v>74</v>
-      </c>
-      <c r="U37" t="s">
-        <v>74</v>
-      </c>
-      <c r="V37" t="s">
-        <v>68</v>
-      </c>
-      <c r="W37" t="s">
-        <v>69</v>
-      </c>
-      <c r="X37" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC37" s="4">
-        <v>39.197000000000003</v>
-      </c>
-      <c r="AD37" s="5">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="AE37" s="5">
-        <v>7.5</v>
-      </c>
-      <c r="AF37" s="5">
-        <v>10.5</v>
-      </c>
-      <c r="AG37" s="5">
-        <v>0.29999999999999999</v>
-      </c>
-      <c r="AH37" s="5">
-        <v>3.7000000000000002</v>
-      </c>
-      <c r="AI37" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="AJ37">
-        <v>55</v>
-      </c>
-      <c r="AK37" s="4">
-        <v>1.5820000000000001</v>
-      </c>
-      <c r="AL37" s="4">
-        <v>1.548</v>
-      </c>
-      <c r="AM37" s="4">
-        <v>1.288</v>
-      </c>
-      <c r="AN37" s="4">
-        <v>0.019</v>
-      </c>
-      <c r="AO37" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="AP37" s="4">
-        <v>0.0070000000000000001</v>
-      </c>
-      <c r="AQ37" s="4">
-        <v>0.0030000000000000001</v>
-      </c>
-      <c r="AR37" s="5">
-        <v>1.3999999999999999</v>
-      </c>
-      <c r="AS37" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>150</v>
-      </c>
-      <c r="B38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F38" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G38" t="s">
-        <v>66</v>
-      </c>
-      <c r="H38" t="s">
-        <v>67</v>
-      </c>
-      <c r="L38" t="s">
-        <v>66</v>
-      </c>
-      <c r="M38" t="s">
-        <v>67</v>
-      </c>
-      <c r="N38" t="s">
-        <v>68</v>
-      </c>
-      <c r="O38" t="s">
-        <v>69</v>
-      </c>
-      <c r="P38" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>71</v>
-      </c>
-      <c r="R38" t="s">
-        <v>72</v>
-      </c>
-      <c r="S38" t="s">
-        <v>73</v>
-      </c>
-      <c r="T38" t="s">
-        <v>74</v>
-      </c>
-      <c r="U38" t="s">
-        <v>74</v>
-      </c>
-      <c r="V38" t="s">
-        <v>68</v>
-      </c>
-      <c r="W38" t="s">
-        <v>69</v>
-      </c>
-      <c r="X38" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z38" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC38" s="4">
-        <v>8.2509999999999994</v>
-      </c>
-      <c r="AD38" s="5">
-        <v>20.899999999999999</v>
-      </c>
-      <c r="AE38" s="5">
-        <v>7.7999999999999998</v>
-      </c>
-      <c r="AF38" s="5">
-        <v>10.800000000000001</v>
-      </c>
-      <c r="AG38" s="5">
-        <v>0.59999999999999998</v>
-      </c>
-      <c r="AH38">
-        <v>2</v>
-      </c>
-      <c r="AI38" s="5">
-        <v>1.3999999999999999</v>
-      </c>
-      <c r="AJ38">
-        <v>80</v>
-      </c>
-      <c r="AK38" s="4">
-        <v>1.589</v>
-      </c>
-      <c r="AL38" s="4">
-        <v>1.5720000000000001</v>
-      </c>
-      <c r="AM38" s="4">
-        <v>1.4530000000000001</v>
-      </c>
-      <c r="AN38" s="4">
-        <v>0.012</v>
-      </c>
-      <c r="AO38" s="4">
-        <v>0.014</v>
-      </c>
-      <c r="AP38" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="AQ38" s="4">
-        <v>0.0060000000000000001</v>
-      </c>
-      <c r="AS38" s="5">
-        <v>0.90000000000000002</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>152</v>
-      </c>
-      <c r="B39" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" t="s">
-        <v>65</v>
-      </c>
-      <c r="E39" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F39" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G39" t="s">
-        <v>66</v>
-      </c>
-      <c r="H39" t="s">
-        <v>67</v>
-      </c>
-      <c r="L39" t="s">
-        <v>66</v>
-      </c>
-      <c r="M39" t="s">
-        <v>67</v>
-      </c>
-      <c r="N39" t="s">
-        <v>68</v>
-      </c>
-      <c r="O39" t="s">
-        <v>69</v>
-      </c>
-      <c r="P39" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>71</v>
-      </c>
-      <c r="R39" t="s">
-        <v>72</v>
-      </c>
-      <c r="S39" t="s">
-        <v>73</v>
-      </c>
-      <c r="T39" t="s">
-        <v>74</v>
-      </c>
-      <c r="U39" t="s">
-        <v>74</v>
-      </c>
-      <c r="V39" t="s">
-        <v>68</v>
-      </c>
-      <c r="W39" t="s">
-        <v>69</v>
-      </c>
-      <c r="X39" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z39" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA39" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>153</v>
-      </c>
-      <c r="AC39" s="4">
-        <v>3.746</v>
-      </c>
-      <c r="AD39" s="5">
-        <v>20.199999999999999</v>
-      </c>
-      <c r="AE39" s="5">
-        <v>7.7999999999999998</v>
-      </c>
-      <c r="AF39" s="5">
-        <v>11.4</v>
-      </c>
-      <c r="AG39" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="AH39" s="5">
-        <v>2.3999999999999999</v>
-      </c>
-      <c r="AI39" s="5">
-        <v>0.80000000000000004</v>
-      </c>
-      <c r="AJ39">
-        <v>98</v>
-      </c>
-      <c r="AK39" s="4">
-        <v>1.6679999999999999</v>
-      </c>
-      <c r="AL39" s="4">
-        <v>1.661</v>
-      </c>
-      <c r="AM39" s="4">
-        <v>1.5609999999999999</v>
-      </c>
-      <c r="AN39" s="4">
-        <v>0.016</v>
-      </c>
-      <c r="AO39" s="4">
-        <v>0.010999999999999999</v>
-      </c>
-      <c r="AP39" s="4">
-        <v>0.0080000000000000002</v>
-      </c>
-      <c r="AQ39" s="4">
-        <v>0.0050000000000000001</v>
-      </c>
-      <c r="AS39" s="5">
-        <v>0.90000000000000002</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>154</v>
-      </c>
-      <c r="B40" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="2">
-        <v>37.828611000000002</v>
-      </c>
-      <c r="F40" s="3">
-        <v>127.51925</v>
-      </c>
-      <c r="G40" t="s">
-        <v>66</v>
-      </c>
-      <c r="H40" t="s">
-        <v>67</v>
-      </c>
-      <c r="L40" t="s">
-        <v>66</v>
-      </c>
-      <c r="M40" t="s">
-        <v>67</v>
-      </c>
-      <c r="N40" t="s">
-        <v>68</v>
-      </c>
-      <c r="O40" t="s">
-        <v>69</v>
-      </c>
-      <c r="P40" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>71</v>
-      </c>
-      <c r="R40" t="s">
-        <v>72</v>
-      </c>
-      <c r="S40" t="s">
-        <v>73</v>
-      </c>
-      <c r="T40" t="s">
-        <v>74</v>
-      </c>
-      <c r="U40" t="s">
-        <v>74</v>
-      </c>
-      <c r="V40" t="s">
-        <v>68</v>
-      </c>
-      <c r="W40" t="s">
-        <v>69</v>
-      </c>
-      <c r="X40" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA40" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB40" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41"/>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>